<commit_message>
update timeline for project
</commit_message>
<xml_diff>
--- a/Empresa/Cronograma_PA.xlsx
+++ b/Empresa/Cronograma_PA.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tiago\Code\DIY-Home-Automation\Empresa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F8621B0E-989F-4452-B545-AB4480692FEB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD26AC36-353B-47FB-B069-A66B047012AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -682,12 +682,84 @@
     <xf numFmtId="0" fontId="5" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="17" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="20" fontId="4" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -709,79 +781,7 @@
     <xf numFmtId="0" fontId="1" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="3" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="3" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="17" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="10" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="10" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="6" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="6" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="7" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="20" fontId="4" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1082,8 +1082,8 @@
   </sheetPr>
   <dimension ref="A2:AP121"/>
   <sheetViews>
-    <sheetView tabSelected="1" showRuler="0" topLeftCell="A70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S108" sqref="S108"/>
+    <sheetView tabSelected="1" showRuler="0" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q97" sqref="Q97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="4.7109375" defaultRowHeight="12.75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1094,43 +1094,43 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C2" s="47" t="s">
+      <c r="C2" s="49" t="s">
         <v>38</v>
       </c>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="M2" s="48"/>
-      <c r="N2" s="48"/>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Y2" s="48"/>
-      <c r="Z2" s="48"/>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="M2" s="50"/>
+      <c r="N2" s="50"/>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Y2" s="50"/>
+      <c r="Z2" s="50"/>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+      <c r="AH2" s="50"/>
     </row>
     <row r="5" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C5" s="57" t="s">
+      <c r="C5" s="56" t="s">
         <v>28</v>
       </c>
       <c r="D5" s="2"/>
@@ -1226,7 +1226,7 @@
       </c>
     </row>
     <row r="6" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C6" s="50"/>
+      <c r="C6" s="52"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2" t="s">
         <v>4</v>
@@ -1385,9 +1385,9 @@
       <c r="AB8" s="3"/>
       <c r="AC8" s="31"/>
       <c r="AD8" s="31"/>
-      <c r="AE8" s="31"/>
+      <c r="AE8" s="30"/>
       <c r="AF8" s="30"/>
-      <c r="AG8" s="30"/>
+      <c r="AG8" s="31"/>
       <c r="AH8" s="3"/>
     </row>
     <row r="9" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1421,9 +1421,9 @@
       <c r="AB9" s="3"/>
       <c r="AC9" s="31"/>
       <c r="AD9" s="31"/>
-      <c r="AE9" s="31"/>
+      <c r="AE9" s="30"/>
       <c r="AF9" s="30"/>
-      <c r="AG9" s="30"/>
+      <c r="AG9" s="31"/>
       <c r="AH9" s="3"/>
     </row>
     <row r="10" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1457,9 +1457,9 @@
       <c r="AB10" s="3"/>
       <c r="AC10" s="31"/>
       <c r="AD10" s="31"/>
-      <c r="AE10" s="31"/>
+      <c r="AE10" s="30"/>
       <c r="AF10" s="30"/>
-      <c r="AG10" s="30"/>
+      <c r="AG10" s="31"/>
       <c r="AH10" s="3"/>
     </row>
     <row r="11" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1493,9 +1493,9 @@
       <c r="AB11" s="3"/>
       <c r="AC11" s="31"/>
       <c r="AD11" s="31"/>
-      <c r="AE11" s="31"/>
+      <c r="AE11" s="30"/>
       <c r="AF11" s="30"/>
-      <c r="AG11" s="30"/>
+      <c r="AG11" s="31"/>
       <c r="AH11" s="3"/>
     </row>
     <row r="12" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1529,9 +1529,9 @@
       <c r="AB12" s="3"/>
       <c r="AC12" s="31"/>
       <c r="AD12" s="31"/>
-      <c r="AE12" s="31"/>
+      <c r="AE12" s="30"/>
       <c r="AF12" s="30"/>
-      <c r="AG12" s="30"/>
+      <c r="AG12" s="31"/>
       <c r="AH12" s="3"/>
     </row>
     <row r="13" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1565,9 +1565,9 @@
       <c r="AB13" s="3"/>
       <c r="AC13" s="31"/>
       <c r="AD13" s="31"/>
-      <c r="AE13" s="31"/>
+      <c r="AE13" s="30"/>
       <c r="AF13" s="30"/>
-      <c r="AG13" s="30"/>
+      <c r="AG13" s="31"/>
       <c r="AH13" s="3"/>
     </row>
     <row r="14" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1601,9 +1601,9 @@
       <c r="AB14" s="3"/>
       <c r="AC14" s="31"/>
       <c r="AD14" s="31"/>
-      <c r="AE14" s="31"/>
+      <c r="AE14" s="30"/>
       <c r="AF14" s="30"/>
-      <c r="AG14" s="30"/>
+      <c r="AG14" s="31"/>
       <c r="AH14" s="3"/>
     </row>
     <row r="15" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1637,9 +1637,9 @@
       <c r="AB15" s="3"/>
       <c r="AC15" s="31"/>
       <c r="AD15" s="31"/>
-      <c r="AE15" s="31"/>
+      <c r="AE15" s="30"/>
       <c r="AF15" s="30"/>
-      <c r="AG15" s="30"/>
+      <c r="AG15" s="31"/>
       <c r="AH15" s="3"/>
     </row>
     <row r="16" spans="2:34" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1673,9 +1673,9 @@
       <c r="AB16" s="3"/>
       <c r="AC16" s="31"/>
       <c r="AD16" s="31"/>
-      <c r="AE16" s="31"/>
+      <c r="AE16" s="30"/>
       <c r="AF16" s="30"/>
-      <c r="AG16" s="30"/>
+      <c r="AG16" s="31"/>
       <c r="AH16" s="3"/>
     </row>
     <row r="17" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1709,9 +1709,9 @@
       <c r="AB17" s="3"/>
       <c r="AC17" s="31"/>
       <c r="AD17" s="31"/>
-      <c r="AE17" s="31"/>
+      <c r="AE17" s="30"/>
       <c r="AF17" s="30"/>
-      <c r="AG17" s="30"/>
+      <c r="AG17" s="31"/>
       <c r="AH17" s="3"/>
     </row>
     <row r="18" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1786,7 +1786,7 @@
       <c r="AG22" s="5"/>
     </row>
     <row r="23" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="49" t="s">
+      <c r="C23" s="51" t="s">
         <v>7</v>
       </c>
       <c r="D23" s="2">
@@ -1889,7 +1889,7 @@
       <c r="AP23" s="1"/>
     </row>
     <row r="24" spans="2:42" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="50"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="2" t="s">
         <v>0</v>
       </c>
@@ -2040,7 +2040,7 @@
       <c r="E26" s="35"/>
       <c r="F26" s="33"/>
       <c r="G26" s="33"/>
-      <c r="H26" s="58" t="s">
+      <c r="H26" s="57" t="s">
         <v>20</v>
       </c>
       <c r="I26" s="30"/>
@@ -2086,7 +2086,7 @@
       <c r="E27" s="35"/>
       <c r="F27" s="33"/>
       <c r="G27" s="33"/>
-      <c r="H27" s="59"/>
+      <c r="H27" s="58"/>
       <c r="I27" s="30"/>
       <c r="J27" s="3"/>
       <c r="K27" s="26"/>
@@ -2130,7 +2130,7 @@
       <c r="E28" s="35"/>
       <c r="F28" s="33"/>
       <c r="G28" s="33"/>
-      <c r="H28" s="59"/>
+      <c r="H28" s="58"/>
       <c r="I28" s="30"/>
       <c r="J28" s="3"/>
       <c r="K28" s="26"/>
@@ -2174,7 +2174,7 @@
       <c r="E29" s="35"/>
       <c r="F29" s="33"/>
       <c r="G29" s="33"/>
-      <c r="H29" s="59"/>
+      <c r="H29" s="58"/>
       <c r="I29" s="30"/>
       <c r="J29" s="3"/>
       <c r="K29" s="26"/>
@@ -2218,7 +2218,7 @@
       <c r="E30" s="35"/>
       <c r="F30" s="33"/>
       <c r="G30" s="33"/>
-      <c r="H30" s="59"/>
+      <c r="H30" s="58"/>
       <c r="I30" s="30"/>
       <c r="J30" s="3"/>
       <c r="K30" s="26"/>
@@ -2262,7 +2262,7 @@
       <c r="E31" s="35"/>
       <c r="F31" s="33"/>
       <c r="G31" s="33"/>
-      <c r="H31" s="59"/>
+      <c r="H31" s="58"/>
       <c r="I31" s="30"/>
       <c r="J31" s="3"/>
       <c r="K31" s="26"/>
@@ -2306,7 +2306,7 @@
       <c r="E32" s="35"/>
       <c r="F32" s="33"/>
       <c r="G32" s="33"/>
-      <c r="H32" s="59"/>
+      <c r="H32" s="58"/>
       <c r="I32" s="30"/>
       <c r="J32" s="3"/>
       <c r="K32" s="26"/>
@@ -2350,7 +2350,7 @@
       <c r="E33" s="35"/>
       <c r="F33" s="33"/>
       <c r="G33" s="33"/>
-      <c r="H33" s="59"/>
+      <c r="H33" s="58"/>
       <c r="I33" s="30"/>
       <c r="J33" s="3"/>
       <c r="K33" s="26"/>
@@ -2394,7 +2394,7 @@
       <c r="E34" s="35"/>
       <c r="F34" s="33"/>
       <c r="G34" s="33"/>
-      <c r="H34" s="59"/>
+      <c r="H34" s="58"/>
       <c r="I34" s="30"/>
       <c r="J34" s="3"/>
       <c r="K34" s="26"/>
@@ -2438,7 +2438,7 @@
       <c r="E35" s="35"/>
       <c r="F35" s="33"/>
       <c r="G35" s="33"/>
-      <c r="H35" s="60"/>
+      <c r="H35" s="59"/>
       <c r="I35" s="30"/>
       <c r="J35" s="3"/>
       <c r="K35" s="26"/>
@@ -2599,7 +2599,7 @@
     </row>
     <row r="39" spans="2:42" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39"/>
-      <c r="C39" s="51" t="s">
+      <c r="C39" s="53" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="2"/>
@@ -2701,7 +2701,7 @@
     </row>
     <row r="40" spans="2:42" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40"/>
-      <c r="C40" s="51"/>
+      <c r="C40" s="53"/>
       <c r="D40" s="2"/>
       <c r="E40" s="2" t="s">
         <v>2</v>
@@ -2800,39 +2800,39 @@
       <c r="AM40" s="8"/>
     </row>
     <row r="41" spans="2:42" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="52"/>
-      <c r="C41" s="52"/>
-      <c r="D41" s="52"/>
-      <c r="E41" s="52"/>
-      <c r="F41" s="52"/>
-      <c r="G41" s="52"/>
-      <c r="H41" s="52"/>
-      <c r="I41" s="52"/>
-      <c r="J41" s="52"/>
-      <c r="K41" s="52"/>
-      <c r="L41" s="52"/>
-      <c r="M41" s="52"/>
-      <c r="N41" s="52"/>
-      <c r="O41" s="52"/>
-      <c r="P41" s="52"/>
-      <c r="Q41" s="52"/>
-      <c r="R41" s="52"/>
-      <c r="S41" s="52"/>
-      <c r="T41" s="52"/>
-      <c r="U41" s="52"/>
-      <c r="V41" s="52"/>
-      <c r="W41" s="52"/>
-      <c r="X41" s="52"/>
-      <c r="Y41" s="52"/>
-      <c r="Z41" s="52"/>
-      <c r="AA41" s="52"/>
-      <c r="AB41" s="52"/>
-      <c r="AC41" s="52"/>
-      <c r="AD41" s="52"/>
-      <c r="AE41" s="52"/>
-      <c r="AF41" s="52"/>
-      <c r="AG41" s="52"/>
-      <c r="AH41" s="52"/>
+      <c r="B41" s="54"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="54"/>
+      <c r="E41" s="54"/>
+      <c r="F41" s="54"/>
+      <c r="G41" s="54"/>
+      <c r="H41" s="54"/>
+      <c r="I41" s="54"/>
+      <c r="J41" s="54"/>
+      <c r="K41" s="54"/>
+      <c r="L41" s="54"/>
+      <c r="M41" s="54"/>
+      <c r="N41" s="54"/>
+      <c r="O41" s="54"/>
+      <c r="P41" s="54"/>
+      <c r="Q41" s="54"/>
+      <c r="R41" s="54"/>
+      <c r="S41" s="54"/>
+      <c r="T41" s="54"/>
+      <c r="U41" s="54"/>
+      <c r="V41" s="54"/>
+      <c r="W41" s="54"/>
+      <c r="X41" s="54"/>
+      <c r="Y41" s="54"/>
+      <c r="Z41" s="54"/>
+      <c r="AA41" s="54"/>
+      <c r="AB41" s="54"/>
+      <c r="AC41" s="54"/>
+      <c r="AD41" s="54"/>
+      <c r="AE41" s="54"/>
+      <c r="AF41" s="54"/>
+      <c r="AG41" s="54"/>
+      <c r="AH41" s="54"/>
       <c r="AI41"/>
       <c r="AJ41"/>
       <c r="AK41"/>
@@ -2844,8 +2844,8 @@
       <c r="C42" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D42" s="54"/>
-      <c r="E42" s="54" t="s">
+      <c r="D42" s="43"/>
+      <c r="E42" s="43" t="s">
         <v>21</v>
       </c>
       <c r="F42" s="29"/>
@@ -2888,8 +2888,8 @@
       <c r="C43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="55"/>
-      <c r="E43" s="55"/>
+      <c r="D43" s="44"/>
+      <c r="E43" s="44"/>
       <c r="F43" s="29"/>
       <c r="G43" s="34"/>
       <c r="H43" s="3"/>
@@ -2930,8 +2930,8 @@
       <c r="C44" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D44" s="55"/>
-      <c r="E44" s="55"/>
+      <c r="D44" s="44"/>
+      <c r="E44" s="44"/>
       <c r="F44" s="29"/>
       <c r="G44" s="34"/>
       <c r="H44" s="3"/>
@@ -2972,8 +2972,8 @@
       <c r="C45" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="55"/>
-      <c r="E45" s="55"/>
+      <c r="D45" s="44"/>
+      <c r="E45" s="44"/>
       <c r="F45" s="29"/>
       <c r="G45" s="34"/>
       <c r="H45" s="3"/>
@@ -3014,8 +3014,8 @@
       <c r="C46" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D46" s="55"/>
-      <c r="E46" s="55"/>
+      <c r="D46" s="44"/>
+      <c r="E46" s="44"/>
       <c r="F46" s="29"/>
       <c r="G46" s="34"/>
       <c r="H46" s="3"/>
@@ -3056,8 +3056,8 @@
       <c r="C47" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D47" s="55"/>
-      <c r="E47" s="55"/>
+      <c r="D47" s="44"/>
+      <c r="E47" s="44"/>
       <c r="F47" s="29"/>
       <c r="G47" s="34"/>
       <c r="H47" s="3"/>
@@ -3098,8 +3098,8 @@
       <c r="C48" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D48" s="55"/>
-      <c r="E48" s="55"/>
+      <c r="D48" s="44"/>
+      <c r="E48" s="44"/>
       <c r="F48" s="29"/>
       <c r="G48" s="34"/>
       <c r="H48" s="3"/>
@@ -3140,8 +3140,8 @@
       <c r="C49" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D49" s="55"/>
-      <c r="E49" s="55"/>
+      <c r="D49" s="44"/>
+      <c r="E49" s="44"/>
       <c r="F49" s="29"/>
       <c r="G49" s="34"/>
       <c r="H49" s="3"/>
@@ -3182,8 +3182,8 @@
       <c r="C50" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D50" s="55"/>
-      <c r="E50" s="55"/>
+      <c r="D50" s="44"/>
+      <c r="E50" s="44"/>
       <c r="F50" s="29"/>
       <c r="G50" s="34"/>
       <c r="H50" s="3"/>
@@ -3224,8 +3224,8 @@
       <c r="C51" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="56"/>
-      <c r="E51" s="56"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
       <c r="F51" s="29"/>
       <c r="G51" s="34"/>
       <c r="H51" s="3"/>
@@ -3262,39 +3262,39 @@
       <c r="AM51"/>
     </row>
     <row r="52" spans="2:39" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B52" s="52"/>
-      <c r="C52" s="52"/>
-      <c r="D52" s="52"/>
-      <c r="E52" s="52"/>
-      <c r="F52" s="52"/>
-      <c r="G52" s="52"/>
-      <c r="H52" s="52"/>
-      <c r="I52" s="52"/>
-      <c r="J52" s="52"/>
-      <c r="K52" s="52"/>
-      <c r="L52" s="52"/>
-      <c r="M52" s="52"/>
-      <c r="N52" s="52"/>
-      <c r="O52" s="52"/>
-      <c r="P52" s="52"/>
-      <c r="Q52" s="52"/>
-      <c r="R52" s="52"/>
-      <c r="S52" s="52"/>
-      <c r="T52" s="52"/>
-      <c r="U52" s="52"/>
-      <c r="V52" s="52"/>
-      <c r="W52" s="52"/>
-      <c r="X52" s="52"/>
-      <c r="Y52" s="52"/>
-      <c r="Z52" s="52"/>
-      <c r="AA52" s="52"/>
-      <c r="AB52" s="52"/>
-      <c r="AC52" s="52"/>
-      <c r="AD52" s="52"/>
-      <c r="AE52" s="52"/>
-      <c r="AF52" s="52"/>
-      <c r="AG52" s="52"/>
-      <c r="AH52" s="52"/>
+      <c r="B52" s="54"/>
+      <c r="C52" s="54"/>
+      <c r="D52" s="54"/>
+      <c r="E52" s="54"/>
+      <c r="F52" s="54"/>
+      <c r="G52" s="54"/>
+      <c r="H52" s="54"/>
+      <c r="I52" s="54"/>
+      <c r="J52" s="54"/>
+      <c r="K52" s="54"/>
+      <c r="L52" s="54"/>
+      <c r="M52" s="54"/>
+      <c r="N52" s="54"/>
+      <c r="O52" s="54"/>
+      <c r="P52" s="54"/>
+      <c r="Q52" s="54"/>
+      <c r="R52" s="54"/>
+      <c r="S52" s="54"/>
+      <c r="T52" s="54"/>
+      <c r="U52" s="54"/>
+      <c r="V52" s="54"/>
+      <c r="W52" s="54"/>
+      <c r="X52" s="54"/>
+      <c r="Y52" s="54"/>
+      <c r="Z52" s="54"/>
+      <c r="AA52" s="54"/>
+      <c r="AB52" s="54"/>
+      <c r="AC52" s="54"/>
+      <c r="AD52" s="54"/>
+      <c r="AE52" s="54"/>
+      <c r="AF52" s="54"/>
+      <c r="AG52" s="54"/>
+      <c r="AH52" s="54"/>
       <c r="AI52"/>
       <c r="AJ52"/>
       <c r="AK52"/>
@@ -3383,7 +3383,7 @@
     </row>
     <row r="55" spans="2:39" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B55"/>
-      <c r="C55" s="51" t="s">
+      <c r="C55" s="53" t="s">
         <v>9</v>
       </c>
       <c r="D55" s="2"/>
@@ -3487,7 +3487,7 @@
     </row>
     <row r="56" spans="2:39" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B56"/>
-      <c r="C56" s="51"/>
+      <c r="C56" s="53"/>
       <c r="D56" s="2"/>
       <c r="E56" s="2" t="s">
         <v>4</v>
@@ -3588,40 +3588,40 @@
       <c r="AM56" s="8"/>
     </row>
     <row r="57" spans="2:39" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B57" s="52"/>
-      <c r="C57" s="52"/>
-      <c r="D57" s="52"/>
-      <c r="E57" s="52"/>
-      <c r="F57" s="52"/>
-      <c r="G57" s="52"/>
-      <c r="H57" s="52"/>
-      <c r="I57" s="52"/>
-      <c r="J57" s="52"/>
-      <c r="K57" s="52"/>
-      <c r="L57" s="52"/>
-      <c r="M57" s="52"/>
-      <c r="N57" s="52"/>
-      <c r="O57" s="52"/>
-      <c r="P57" s="52"/>
-      <c r="Q57" s="52"/>
-      <c r="R57" s="52"/>
-      <c r="S57" s="52"/>
-      <c r="T57" s="52"/>
-      <c r="U57" s="52"/>
-      <c r="V57" s="52"/>
-      <c r="W57" s="52"/>
-      <c r="X57" s="52"/>
-      <c r="Y57" s="52"/>
-      <c r="Z57" s="52"/>
-      <c r="AA57" s="52"/>
-      <c r="AB57" s="52"/>
-      <c r="AC57" s="52"/>
-      <c r="AD57" s="52"/>
-      <c r="AE57" s="52"/>
-      <c r="AF57" s="52"/>
-      <c r="AG57" s="52"/>
-      <c r="AH57" s="52"/>
-      <c r="AI57" s="52"/>
+      <c r="B57" s="54"/>
+      <c r="C57" s="54"/>
+      <c r="D57" s="54"/>
+      <c r="E57" s="54"/>
+      <c r="F57" s="54"/>
+      <c r="G57" s="54"/>
+      <c r="H57" s="54"/>
+      <c r="I57" s="54"/>
+      <c r="J57" s="54"/>
+      <c r="K57" s="54"/>
+      <c r="L57" s="54"/>
+      <c r="M57" s="54"/>
+      <c r="N57" s="54"/>
+      <c r="O57" s="54"/>
+      <c r="P57" s="54"/>
+      <c r="Q57" s="54"/>
+      <c r="R57" s="54"/>
+      <c r="S57" s="54"/>
+      <c r="T57" s="54"/>
+      <c r="U57" s="54"/>
+      <c r="V57" s="54"/>
+      <c r="W57" s="54"/>
+      <c r="X57" s="54"/>
+      <c r="Y57" s="54"/>
+      <c r="Z57" s="54"/>
+      <c r="AA57" s="54"/>
+      <c r="AB57" s="54"/>
+      <c r="AC57" s="54"/>
+      <c r="AD57" s="54"/>
+      <c r="AE57" s="54"/>
+      <c r="AF57" s="54"/>
+      <c r="AG57" s="54"/>
+      <c r="AH57" s="54"/>
+      <c r="AI57" s="54"/>
       <c r="AJ57" s="8"/>
       <c r="AK57" s="8"/>
       <c r="AL57" s="8"/>
@@ -3632,8 +3632,8 @@
       <c r="C58" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D58" s="54"/>
-      <c r="E58" s="54" t="s">
+      <c r="D58" s="43"/>
+      <c r="E58" s="43" t="s">
         <v>22</v>
       </c>
       <c r="F58" s="3"/>
@@ -3642,7 +3642,7 @@
       <c r="I58" s="36"/>
       <c r="J58" s="36"/>
       <c r="K58" s="34"/>
-      <c r="L58" s="54" t="s">
+      <c r="L58" s="43" t="s">
         <v>23</v>
       </c>
       <c r="M58" s="3"/>
@@ -3655,21 +3655,21 @@
       <c r="T58" s="3"/>
       <c r="U58" s="3"/>
       <c r="V58" s="34"/>
-      <c r="W58" s="67" t="s">
+      <c r="W58" s="46" t="s">
         <v>25</v>
       </c>
       <c r="X58" s="20"/>
       <c r="Y58" s="20"/>
       <c r="Z58" s="20"/>
       <c r="AA58" s="20"/>
-      <c r="AB58" s="64"/>
-      <c r="AC58" s="54" t="s">
+      <c r="AB58" s="40"/>
+      <c r="AC58" s="43" t="s">
         <v>24</v>
       </c>
-      <c r="AD58" s="64"/>
-      <c r="AE58" s="64"/>
-      <c r="AF58" s="64"/>
-      <c r="AG58" s="64"/>
+      <c r="AD58" s="40"/>
+      <c r="AE58" s="40"/>
+      <c r="AF58" s="40"/>
+      <c r="AG58" s="40"/>
       <c r="AH58" s="3"/>
       <c r="AI58" s="3"/>
       <c r="AJ58" s="8"/>
@@ -3682,15 +3682,15 @@
       <c r="C59" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="55"/>
-      <c r="E59" s="55"/>
+      <c r="D59" s="44"/>
+      <c r="E59" s="44"/>
       <c r="F59" s="3"/>
       <c r="G59" s="3"/>
       <c r="H59" s="36"/>
       <c r="I59" s="36"/>
       <c r="J59" s="36"/>
       <c r="K59" s="34"/>
-      <c r="L59" s="55"/>
+      <c r="L59" s="44"/>
       <c r="M59" s="3"/>
       <c r="N59" s="3"/>
       <c r="O59" s="34"/>
@@ -3701,17 +3701,17 @@
       <c r="T59" s="3"/>
       <c r="U59" s="3"/>
       <c r="V59" s="34"/>
-      <c r="W59" s="68"/>
+      <c r="W59" s="47"/>
       <c r="X59" s="21"/>
       <c r="Y59" s="21"/>
       <c r="Z59" s="21"/>
       <c r="AA59" s="21"/>
-      <c r="AB59" s="65"/>
-      <c r="AC59" s="55"/>
-      <c r="AD59" s="65"/>
-      <c r="AE59" s="65"/>
-      <c r="AF59" s="65"/>
-      <c r="AG59" s="65"/>
+      <c r="AB59" s="41"/>
+      <c r="AC59" s="44"/>
+      <c r="AD59" s="41"/>
+      <c r="AE59" s="41"/>
+      <c r="AF59" s="41"/>
+      <c r="AG59" s="41"/>
       <c r="AH59" s="3"/>
       <c r="AI59" s="3"/>
       <c r="AJ59" s="8"/>
@@ -3724,15 +3724,15 @@
       <c r="C60" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D60" s="55"/>
-      <c r="E60" s="55"/>
+      <c r="D60" s="44"/>
+      <c r="E60" s="44"/>
       <c r="F60" s="3"/>
       <c r="G60" s="3"/>
       <c r="H60" s="36"/>
       <c r="I60" s="36"/>
       <c r="J60" s="36"/>
       <c r="K60" s="34"/>
-      <c r="L60" s="55"/>
+      <c r="L60" s="44"/>
       <c r="M60" s="3"/>
       <c r="N60" s="3"/>
       <c r="O60" s="34"/>
@@ -3743,17 +3743,17 @@
       <c r="T60" s="3"/>
       <c r="U60" s="3"/>
       <c r="V60" s="34"/>
-      <c r="W60" s="68"/>
+      <c r="W60" s="47"/>
       <c r="X60" s="21"/>
       <c r="Y60" s="21"/>
       <c r="Z60" s="21"/>
       <c r="AA60" s="21"/>
-      <c r="AB60" s="65"/>
-      <c r="AC60" s="55"/>
-      <c r="AD60" s="65"/>
-      <c r="AE60" s="65"/>
-      <c r="AF60" s="65"/>
-      <c r="AG60" s="65"/>
+      <c r="AB60" s="41"/>
+      <c r="AC60" s="44"/>
+      <c r="AD60" s="41"/>
+      <c r="AE60" s="41"/>
+      <c r="AF60" s="41"/>
+      <c r="AG60" s="41"/>
       <c r="AH60" s="3"/>
       <c r="AI60" s="3"/>
       <c r="AJ60" s="8"/>
@@ -3766,15 +3766,15 @@
       <c r="C61" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D61" s="55"/>
-      <c r="E61" s="55"/>
+      <c r="D61" s="44"/>
+      <c r="E61" s="44"/>
       <c r="F61" s="3"/>
       <c r="G61" s="3"/>
       <c r="H61" s="36"/>
       <c r="I61" s="36"/>
       <c r="J61" s="36"/>
       <c r="K61" s="34"/>
-      <c r="L61" s="55"/>
+      <c r="L61" s="44"/>
       <c r="M61" s="3"/>
       <c r="N61" s="3"/>
       <c r="O61" s="34"/>
@@ -3785,17 +3785,17 @@
       <c r="T61" s="3"/>
       <c r="U61" s="3"/>
       <c r="V61" s="34"/>
-      <c r="W61" s="68"/>
+      <c r="W61" s="47"/>
       <c r="X61" s="21"/>
       <c r="Y61" s="21"/>
       <c r="Z61" s="21"/>
       <c r="AA61" s="21"/>
-      <c r="AB61" s="65"/>
-      <c r="AC61" s="55"/>
-      <c r="AD61" s="65"/>
-      <c r="AE61" s="65"/>
-      <c r="AF61" s="65"/>
-      <c r="AG61" s="65"/>
+      <c r="AB61" s="41"/>
+      <c r="AC61" s="44"/>
+      <c r="AD61" s="41"/>
+      <c r="AE61" s="41"/>
+      <c r="AF61" s="41"/>
+      <c r="AG61" s="41"/>
       <c r="AH61" s="3"/>
       <c r="AI61" s="3"/>
       <c r="AJ61" s="8"/>
@@ -3808,15 +3808,15 @@
       <c r="C62" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D62" s="55"/>
-      <c r="E62" s="55"/>
+      <c r="D62" s="44"/>
+      <c r="E62" s="44"/>
       <c r="F62" s="3"/>
       <c r="G62" s="3"/>
       <c r="H62" s="36"/>
       <c r="I62" s="36"/>
       <c r="J62" s="36"/>
       <c r="K62" s="34"/>
-      <c r="L62" s="55"/>
+      <c r="L62" s="44"/>
       <c r="M62" s="3"/>
       <c r="N62" s="3"/>
       <c r="O62" s="34"/>
@@ -3827,17 +3827,17 @@
       <c r="T62" s="3"/>
       <c r="U62" s="3"/>
       <c r="V62" s="34"/>
-      <c r="W62" s="68"/>
+      <c r="W62" s="47"/>
       <c r="X62" s="21"/>
       <c r="Y62" s="21"/>
       <c r="Z62" s="21"/>
       <c r="AA62" s="21"/>
-      <c r="AB62" s="65"/>
-      <c r="AC62" s="55"/>
-      <c r="AD62" s="65"/>
-      <c r="AE62" s="65"/>
-      <c r="AF62" s="65"/>
-      <c r="AG62" s="65"/>
+      <c r="AB62" s="41"/>
+      <c r="AC62" s="44"/>
+      <c r="AD62" s="41"/>
+      <c r="AE62" s="41"/>
+      <c r="AF62" s="41"/>
+      <c r="AG62" s="41"/>
       <c r="AH62" s="3"/>
       <c r="AI62" s="3"/>
       <c r="AJ62" s="8"/>
@@ -3850,15 +3850,15 @@
       <c r="C63" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D63" s="55"/>
-      <c r="E63" s="55"/>
+      <c r="D63" s="44"/>
+      <c r="E63" s="44"/>
       <c r="F63" s="3"/>
       <c r="G63" s="3"/>
       <c r="H63" s="36"/>
       <c r="I63" s="36"/>
       <c r="J63" s="36"/>
       <c r="K63" s="34"/>
-      <c r="L63" s="55"/>
+      <c r="L63" s="44"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
       <c r="O63" s="34"/>
@@ -3869,17 +3869,17 @@
       <c r="T63" s="3"/>
       <c r="U63" s="3"/>
       <c r="V63" s="34"/>
-      <c r="W63" s="68"/>
+      <c r="W63" s="47"/>
       <c r="X63" s="21"/>
       <c r="Y63" s="21"/>
       <c r="Z63" s="21"/>
       <c r="AA63" s="21"/>
-      <c r="AB63" s="65"/>
-      <c r="AC63" s="55"/>
-      <c r="AD63" s="65"/>
-      <c r="AE63" s="65"/>
-      <c r="AF63" s="65"/>
-      <c r="AG63" s="65"/>
+      <c r="AB63" s="41"/>
+      <c r="AC63" s="44"/>
+      <c r="AD63" s="41"/>
+      <c r="AE63" s="41"/>
+      <c r="AF63" s="41"/>
+      <c r="AG63" s="41"/>
       <c r="AH63" s="3"/>
       <c r="AI63" s="3"/>
       <c r="AJ63" s="8"/>
@@ -3892,15 +3892,15 @@
       <c r="C64" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D64" s="55"/>
-      <c r="E64" s="55"/>
+      <c r="D64" s="44"/>
+      <c r="E64" s="44"/>
       <c r="F64" s="3"/>
       <c r="G64" s="3"/>
       <c r="H64" s="36"/>
       <c r="I64" s="36"/>
       <c r="J64" s="36"/>
       <c r="K64" s="34"/>
-      <c r="L64" s="55"/>
+      <c r="L64" s="44"/>
       <c r="M64" s="3"/>
       <c r="N64" s="3"/>
       <c r="O64" s="34"/>
@@ -3911,17 +3911,17 @@
       <c r="T64" s="3"/>
       <c r="U64" s="3"/>
       <c r="V64" s="34"/>
-      <c r="W64" s="68"/>
+      <c r="W64" s="47"/>
       <c r="X64" s="21"/>
       <c r="Y64" s="21"/>
       <c r="Z64" s="21"/>
       <c r="AA64" s="21"/>
-      <c r="AB64" s="65"/>
-      <c r="AC64" s="55"/>
-      <c r="AD64" s="65"/>
-      <c r="AE64" s="65"/>
-      <c r="AF64" s="65"/>
-      <c r="AG64" s="65"/>
+      <c r="AB64" s="41"/>
+      <c r="AC64" s="44"/>
+      <c r="AD64" s="41"/>
+      <c r="AE64" s="41"/>
+      <c r="AF64" s="41"/>
+      <c r="AG64" s="41"/>
       <c r="AH64" s="3"/>
       <c r="AI64" s="3"/>
       <c r="AJ64" s="8"/>
@@ -3934,15 +3934,15 @@
       <c r="C65" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D65" s="55"/>
-      <c r="E65" s="55"/>
+      <c r="D65" s="44"/>
+      <c r="E65" s="44"/>
       <c r="F65" s="3"/>
       <c r="G65" s="3"/>
       <c r="H65" s="36"/>
       <c r="I65" s="36"/>
       <c r="J65" s="36"/>
       <c r="K65" s="34"/>
-      <c r="L65" s="55"/>
+      <c r="L65" s="44"/>
       <c r="M65" s="3"/>
       <c r="N65" s="3"/>
       <c r="O65" s="34"/>
@@ -3953,17 +3953,17 @@
       <c r="T65" s="3"/>
       <c r="U65" s="3"/>
       <c r="V65" s="34"/>
-      <c r="W65" s="68"/>
+      <c r="W65" s="47"/>
       <c r="X65" s="21"/>
       <c r="Y65" s="21"/>
       <c r="Z65" s="21"/>
       <c r="AA65" s="21"/>
-      <c r="AB65" s="65"/>
-      <c r="AC65" s="55"/>
-      <c r="AD65" s="65"/>
-      <c r="AE65" s="65"/>
-      <c r="AF65" s="65"/>
-      <c r="AG65" s="65"/>
+      <c r="AB65" s="41"/>
+      <c r="AC65" s="44"/>
+      <c r="AD65" s="41"/>
+      <c r="AE65" s="41"/>
+      <c r="AF65" s="41"/>
+      <c r="AG65" s="41"/>
       <c r="AH65" s="3"/>
       <c r="AI65" s="3"/>
       <c r="AJ65" s="8"/>
@@ -3976,15 +3976,15 @@
       <c r="C66" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D66" s="55"/>
-      <c r="E66" s="55"/>
+      <c r="D66" s="44"/>
+      <c r="E66" s="44"/>
       <c r="F66" s="3"/>
       <c r="G66" s="3"/>
       <c r="H66" s="36"/>
       <c r="I66" s="36"/>
       <c r="J66" s="36"/>
       <c r="K66" s="34"/>
-      <c r="L66" s="55"/>
+      <c r="L66" s="44"/>
       <c r="M66" s="3"/>
       <c r="N66" s="3"/>
       <c r="O66" s="34"/>
@@ -3995,17 +3995,17 @@
       <c r="T66" s="3"/>
       <c r="U66" s="3"/>
       <c r="V66" s="34"/>
-      <c r="W66" s="68"/>
+      <c r="W66" s="47"/>
       <c r="X66" s="21"/>
       <c r="Y66" s="21"/>
       <c r="Z66" s="21"/>
       <c r="AA66" s="21"/>
-      <c r="AB66" s="65"/>
-      <c r="AC66" s="55"/>
-      <c r="AD66" s="65"/>
-      <c r="AE66" s="65"/>
-      <c r="AF66" s="65"/>
-      <c r="AG66" s="65"/>
+      <c r="AB66" s="41"/>
+      <c r="AC66" s="44"/>
+      <c r="AD66" s="41"/>
+      <c r="AE66" s="41"/>
+      <c r="AF66" s="41"/>
+      <c r="AG66" s="41"/>
       <c r="AH66" s="3"/>
       <c r="AI66" s="3"/>
       <c r="AJ66" s="8"/>
@@ -4018,15 +4018,15 @@
       <c r="C67" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D67" s="56"/>
-      <c r="E67" s="56"/>
+      <c r="D67" s="45"/>
+      <c r="E67" s="45"/>
       <c r="F67" s="3"/>
       <c r="G67" s="3"/>
       <c r="H67" s="36"/>
       <c r="I67" s="36"/>
       <c r="J67" s="36"/>
       <c r="K67" s="34"/>
-      <c r="L67" s="56"/>
+      <c r="L67" s="45"/>
       <c r="M67" s="3"/>
       <c r="N67" s="3"/>
       <c r="O67" s="34"/>
@@ -4037,17 +4037,17 @@
       <c r="T67" s="3"/>
       <c r="U67" s="3"/>
       <c r="V67" s="34"/>
-      <c r="W67" s="69"/>
+      <c r="W67" s="48"/>
       <c r="X67" s="22"/>
       <c r="Y67" s="22"/>
       <c r="Z67" s="22"/>
       <c r="AA67" s="22"/>
-      <c r="AB67" s="66"/>
-      <c r="AC67" s="56"/>
-      <c r="AD67" s="66"/>
-      <c r="AE67" s="66"/>
-      <c r="AF67" s="66"/>
-      <c r="AG67" s="66"/>
+      <c r="AB67" s="42"/>
+      <c r="AC67" s="45"/>
+      <c r="AD67" s="42"/>
+      <c r="AE67" s="42"/>
+      <c r="AF67" s="42"/>
+      <c r="AG67" s="42"/>
       <c r="AH67" s="3"/>
       <c r="AI67" s="3"/>
       <c r="AJ67" s="8"/>
@@ -4057,39 +4057,39 @@
     </row>
     <row r="68" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B68" s="23"/>
-      <c r="C68" s="61"/>
-      <c r="D68" s="61"/>
-      <c r="E68" s="61"/>
-      <c r="F68" s="61"/>
-      <c r="G68" s="61"/>
-      <c r="H68" s="61"/>
-      <c r="I68" s="61"/>
-      <c r="J68" s="61"/>
-      <c r="K68" s="61"/>
-      <c r="L68" s="61"/>
-      <c r="M68" s="61"/>
-      <c r="N68" s="61"/>
-      <c r="O68" s="61"/>
-      <c r="P68" s="61"/>
-      <c r="Q68" s="61"/>
-      <c r="R68" s="61"/>
-      <c r="S68" s="61"/>
-      <c r="T68" s="61"/>
-      <c r="U68" s="61"/>
-      <c r="V68" s="61"/>
-      <c r="W68" s="61"/>
-      <c r="X68" s="61"/>
-      <c r="Y68" s="61"/>
-      <c r="Z68" s="61"/>
-      <c r="AA68" s="61"/>
-      <c r="AB68" s="61"/>
-      <c r="AC68" s="61"/>
-      <c r="AD68" s="61"/>
-      <c r="AE68" s="61"/>
-      <c r="AF68" s="61"/>
-      <c r="AG68" s="61"/>
-      <c r="AH68" s="61"/>
-      <c r="AI68" s="61"/>
+      <c r="C68" s="60"/>
+      <c r="D68" s="60"/>
+      <c r="E68" s="60"/>
+      <c r="F68" s="60"/>
+      <c r="G68" s="60"/>
+      <c r="H68" s="60"/>
+      <c r="I68" s="60"/>
+      <c r="J68" s="60"/>
+      <c r="K68" s="60"/>
+      <c r="L68" s="60"/>
+      <c r="M68" s="60"/>
+      <c r="N68" s="60"/>
+      <c r="O68" s="60"/>
+      <c r="P68" s="60"/>
+      <c r="Q68" s="60"/>
+      <c r="R68" s="60"/>
+      <c r="S68" s="60"/>
+      <c r="T68" s="60"/>
+      <c r="U68" s="60"/>
+      <c r="V68" s="60"/>
+      <c r="W68" s="60"/>
+      <c r="X68" s="60"/>
+      <c r="Y68" s="60"/>
+      <c r="Z68" s="60"/>
+      <c r="AA68" s="60"/>
+      <c r="AB68" s="60"/>
+      <c r="AC68" s="60"/>
+      <c r="AD68" s="60"/>
+      <c r="AE68" s="60"/>
+      <c r="AF68" s="60"/>
+      <c r="AG68" s="60"/>
+      <c r="AH68" s="60"/>
+      <c r="AI68" s="60"/>
       <c r="AJ68" s="8"/>
       <c r="AK68" s="8"/>
       <c r="AL68" s="8"/>
@@ -4179,7 +4179,7 @@
     <row r="71" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71"/>
       <c r="B71"/>
-      <c r="C71" s="51" t="s">
+      <c r="C71" s="53" t="s">
         <v>26</v>
       </c>
       <c r="D71" s="2">
@@ -4284,7 +4284,7 @@
     <row r="72" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A72"/>
       <c r="B72"/>
-      <c r="C72" s="51"/>
+      <c r="C72" s="53"/>
       <c r="D72" s="2" t="s">
         <v>0</v>
       </c>
@@ -4386,39 +4386,39 @@
     </row>
     <row r="73" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A73"/>
-      <c r="B73" s="52"/>
-      <c r="C73" s="52"/>
-      <c r="D73" s="52"/>
-      <c r="E73" s="52"/>
-      <c r="F73" s="52"/>
-      <c r="G73" s="52"/>
-      <c r="H73" s="52"/>
-      <c r="I73" s="52"/>
-      <c r="J73" s="52"/>
-      <c r="K73" s="52"/>
-      <c r="L73" s="52"/>
-      <c r="M73" s="52"/>
-      <c r="N73" s="52"/>
-      <c r="O73" s="52"/>
-      <c r="P73" s="52"/>
-      <c r="Q73" s="52"/>
-      <c r="R73" s="52"/>
-      <c r="S73" s="52"/>
-      <c r="T73" s="52"/>
-      <c r="U73" s="52"/>
-      <c r="V73" s="52"/>
-      <c r="W73" s="52"/>
-      <c r="X73" s="52"/>
-      <c r="Y73" s="52"/>
-      <c r="Z73" s="52"/>
-      <c r="AA73" s="52"/>
-      <c r="AB73" s="52"/>
-      <c r="AC73" s="52"/>
-      <c r="AD73" s="52"/>
-      <c r="AE73" s="52"/>
-      <c r="AF73" s="52"/>
-      <c r="AG73" s="52"/>
-      <c r="AH73" s="53"/>
+      <c r="B73" s="54"/>
+      <c r="C73" s="54"/>
+      <c r="D73" s="54"/>
+      <c r="E73" s="54"/>
+      <c r="F73" s="54"/>
+      <c r="G73" s="54"/>
+      <c r="H73" s="54"/>
+      <c r="I73" s="54"/>
+      <c r="J73" s="54"/>
+      <c r="K73" s="54"/>
+      <c r="L73" s="54"/>
+      <c r="M73" s="54"/>
+      <c r="N73" s="54"/>
+      <c r="O73" s="54"/>
+      <c r="P73" s="54"/>
+      <c r="Q73" s="54"/>
+      <c r="R73" s="54"/>
+      <c r="S73" s="54"/>
+      <c r="T73" s="54"/>
+      <c r="U73" s="54"/>
+      <c r="V73" s="54"/>
+      <c r="W73" s="54"/>
+      <c r="X73" s="54"/>
+      <c r="Y73" s="54"/>
+      <c r="Z73" s="54"/>
+      <c r="AA73" s="54"/>
+      <c r="AB73" s="54"/>
+      <c r="AC73" s="54"/>
+      <c r="AD73" s="54"/>
+      <c r="AE73" s="54"/>
+      <c r="AF73" s="54"/>
+      <c r="AG73" s="54"/>
+      <c r="AH73" s="55"/>
       <c r="AI73"/>
       <c r="AJ73"/>
       <c r="AK73"/>
@@ -4432,10 +4432,10 @@
       <c r="C74" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D74" s="54" t="s">
+      <c r="D74" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="E74" s="64"/>
+      <c r="E74" s="40"/>
       <c r="F74" s="3"/>
       <c r="G74" s="19"/>
       <c r="H74" s="27"/>
@@ -4478,8 +4478,8 @@
       <c r="C75" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D75" s="55"/>
-      <c r="E75" s="65"/>
+      <c r="D75" s="44"/>
+      <c r="E75" s="41"/>
       <c r="F75" s="3"/>
       <c r="G75" s="19"/>
       <c r="H75" s="27"/>
@@ -4522,8 +4522,8 @@
       <c r="C76" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D76" s="55"/>
-      <c r="E76" s="65"/>
+      <c r="D76" s="44"/>
+      <c r="E76" s="41"/>
       <c r="F76" s="3"/>
       <c r="G76" s="19"/>
       <c r="H76" s="27"/>
@@ -4566,8 +4566,8 @@
       <c r="C77" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D77" s="55"/>
-      <c r="E77" s="65"/>
+      <c r="D77" s="44"/>
+      <c r="E77" s="41"/>
       <c r="F77" s="3"/>
       <c r="G77" s="19"/>
       <c r="H77" s="27"/>
@@ -4610,8 +4610,8 @@
       <c r="C78" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="D78" s="55"/>
-      <c r="E78" s="65"/>
+      <c r="D78" s="44"/>
+      <c r="E78" s="41"/>
       <c r="F78" s="3"/>
       <c r="G78" s="19"/>
       <c r="H78" s="27"/>
@@ -4654,8 +4654,8 @@
       <c r="C79" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D79" s="55"/>
-      <c r="E79" s="65"/>
+      <c r="D79" s="44"/>
+      <c r="E79" s="41"/>
       <c r="F79" s="3"/>
       <c r="G79" s="19"/>
       <c r="H79" s="27"/>
@@ -4698,8 +4698,8 @@
       <c r="C80" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="D80" s="55"/>
-      <c r="E80" s="65"/>
+      <c r="D80" s="44"/>
+      <c r="E80" s="41"/>
       <c r="F80" s="3"/>
       <c r="G80" s="19"/>
       <c r="H80" s="27"/>
@@ -4742,8 +4742,8 @@
       <c r="C81" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="D81" s="55"/>
-      <c r="E81" s="65"/>
+      <c r="D81" s="44"/>
+      <c r="E81" s="41"/>
       <c r="F81" s="3"/>
       <c r="G81" s="19"/>
       <c r="H81" s="27"/>
@@ -4786,8 +4786,8 @@
       <c r="C82" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D82" s="55"/>
-      <c r="E82" s="65"/>
+      <c r="D82" s="44"/>
+      <c r="E82" s="41"/>
       <c r="F82" s="3"/>
       <c r="G82" s="19"/>
       <c r="H82" s="27"/>
@@ -4830,8 +4830,8 @@
       <c r="C83" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="D83" s="56"/>
-      <c r="E83" s="66"/>
+      <c r="D83" s="45"/>
+      <c r="E83" s="42"/>
       <c r="F83" s="3"/>
       <c r="G83" s="19"/>
       <c r="H83" s="27"/>
@@ -4870,39 +4870,39 @@
     </row>
     <row r="84" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A84"/>
-      <c r="B84" s="62"/>
-      <c r="C84" s="62"/>
-      <c r="D84" s="62"/>
-      <c r="E84" s="62"/>
-      <c r="F84" s="62"/>
-      <c r="G84" s="62"/>
-      <c r="H84" s="62"/>
-      <c r="I84" s="62"/>
-      <c r="J84" s="62"/>
-      <c r="K84" s="62"/>
-      <c r="L84" s="62"/>
-      <c r="M84" s="62"/>
-      <c r="N84" s="62"/>
-      <c r="O84" s="62"/>
-      <c r="P84" s="62"/>
-      <c r="Q84" s="62"/>
-      <c r="R84" s="62"/>
-      <c r="S84" s="62"/>
-      <c r="T84" s="62"/>
-      <c r="U84" s="62"/>
-      <c r="V84" s="62"/>
-      <c r="W84" s="62"/>
-      <c r="X84" s="62"/>
-      <c r="Y84" s="62"/>
-      <c r="Z84" s="62"/>
-      <c r="AA84" s="62"/>
-      <c r="AB84" s="62"/>
-      <c r="AC84" s="62"/>
-      <c r="AD84" s="62"/>
-      <c r="AE84" s="62"/>
-      <c r="AF84" s="62"/>
-      <c r="AG84" s="62"/>
-      <c r="AH84" s="63"/>
+      <c r="B84" s="38"/>
+      <c r="C84" s="38"/>
+      <c r="D84" s="38"/>
+      <c r="E84" s="38"/>
+      <c r="F84" s="38"/>
+      <c r="G84" s="38"/>
+      <c r="H84" s="38"/>
+      <c r="I84" s="38"/>
+      <c r="J84" s="38"/>
+      <c r="K84" s="38"/>
+      <c r="L84" s="38"/>
+      <c r="M84" s="38"/>
+      <c r="N84" s="38"/>
+      <c r="O84" s="38"/>
+      <c r="P84" s="38"/>
+      <c r="Q84" s="38"/>
+      <c r="R84" s="38"/>
+      <c r="S84" s="38"/>
+      <c r="T84" s="38"/>
+      <c r="U84" s="38"/>
+      <c r="V84" s="38"/>
+      <c r="W84" s="38"/>
+      <c r="X84" s="38"/>
+      <c r="Y84" s="38"/>
+      <c r="Z84" s="38"/>
+      <c r="AA84" s="38"/>
+      <c r="AB84" s="38"/>
+      <c r="AC84" s="38"/>
+      <c r="AD84" s="38"/>
+      <c r="AE84" s="38"/>
+      <c r="AF84" s="38"/>
+      <c r="AG84" s="38"/>
+      <c r="AH84" s="39"/>
       <c r="AI84"/>
       <c r="AJ84"/>
       <c r="AK84"/>
@@ -4984,50 +4984,50 @@
     <row r="89" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A89"/>
       <c r="B89"/>
-      <c r="C89" s="46" t="s">
+      <c r="C89" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="D89" s="46"/>
-      <c r="E89" s="46"/>
-      <c r="F89" s="46"/>
-      <c r="G89" s="46"/>
-      <c r="H89" s="46"/>
+      <c r="D89" s="61"/>
+      <c r="E89" s="61"/>
+      <c r="F89" s="61"/>
+      <c r="G89" s="61"/>
+      <c r="H89" s="61"/>
     </row>
     <row r="90" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A90"/>
       <c r="B90"/>
-      <c r="C90" s="37" t="s">
+      <c r="C90" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="37"/>
-      <c r="G90" s="39"/>
-      <c r="H90" s="39"/>
+      <c r="D90" s="62"/>
+      <c r="E90" s="62"/>
+      <c r="F90" s="62"/>
+      <c r="G90" s="63"/>
+      <c r="H90" s="63"/>
     </row>
     <row r="91" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A91"/>
       <c r="B91"/>
-      <c r="C91" s="37" t="s">
+      <c r="C91" s="62" t="s">
         <v>40</v>
       </c>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="37"/>
-      <c r="G91" s="40"/>
-      <c r="H91" s="40"/>
+      <c r="D91" s="62"/>
+      <c r="E91" s="62"/>
+      <c r="F91" s="62"/>
+      <c r="G91" s="64"/>
+      <c r="H91" s="64"/>
     </row>
     <row r="92" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92"/>
       <c r="B92"/>
-      <c r="C92" s="37" t="s">
+      <c r="C92" s="62" t="s">
         <v>42</v>
       </c>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="37"/>
-      <c r="G92" s="41"/>
-      <c r="H92" s="41"/>
+      <c r="D92" s="62"/>
+      <c r="E92" s="62"/>
+      <c r="F92" s="62"/>
+      <c r="G92" s="65"/>
+      <c r="H92" s="65"/>
       <c r="I92" s="32" t="s">
         <v>53</v>
       </c>
@@ -5035,108 +5035,108 @@
     <row r="93" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A93"/>
       <c r="B93"/>
-      <c r="C93" s="37" t="s">
+      <c r="C93" s="62" t="s">
         <v>44</v>
       </c>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="37"/>
-      <c r="G93" s="42"/>
-      <c r="H93" s="42"/>
+      <c r="D93" s="62"/>
+      <c r="E93" s="62"/>
+      <c r="F93" s="62"/>
+      <c r="G93" s="66"/>
+      <c r="H93" s="66"/>
     </row>
     <row r="94" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A94"/>
       <c r="B94"/>
-      <c r="C94" s="37" t="s">
+      <c r="C94" s="62" t="s">
         <v>45</v>
       </c>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="37"/>
-      <c r="G94" s="43"/>
-      <c r="H94" s="43"/>
+      <c r="D94" s="62"/>
+      <c r="E94" s="62"/>
+      <c r="F94" s="62"/>
+      <c r="G94" s="67"/>
+      <c r="H94" s="67"/>
     </row>
     <row r="95" spans="1:40" s="7" customFormat="1" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A95"/>
       <c r="B95"/>
-      <c r="C95" s="37" t="s">
+      <c r="C95" s="62" t="s">
         <v>46</v>
       </c>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="37"/>
-      <c r="G95" s="44"/>
-      <c r="H95" s="44"/>
+      <c r="D95" s="62"/>
+      <c r="E95" s="62"/>
+      <c r="F95" s="62"/>
+      <c r="G95" s="68"/>
+      <c r="H95" s="68"/>
     </row>
     <row r="96" spans="1:40" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A96"/>
       <c r="B96"/>
-      <c r="C96" s="37" t="s">
+      <c r="C96" s="62" t="s">
         <v>43</v>
       </c>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="37"/>
-      <c r="G96" s="45"/>
-      <c r="H96" s="45"/>
+      <c r="D96" s="62"/>
+      <c r="E96" s="62"/>
+      <c r="F96" s="62"/>
+      <c r="G96" s="69"/>
+      <c r="H96" s="69"/>
     </row>
     <row r="97" spans="1:35" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A97"/>
       <c r="B97"/>
-      <c r="C97" s="37" t="s">
+      <c r="C97" s="62" t="s">
         <v>47</v>
       </c>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="37"/>
-      <c r="G97" s="38"/>
-      <c r="H97" s="38"/>
+      <c r="D97" s="62"/>
+      <c r="E97" s="62"/>
+      <c r="F97" s="62"/>
+      <c r="G97" s="70"/>
+      <c r="H97" s="70"/>
     </row>
     <row r="98" spans="1:35" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A98"/>
       <c r="B98"/>
-      <c r="C98" s="37" t="s">
+      <c r="C98" s="62" t="s">
         <v>48</v>
       </c>
-      <c r="D98" s="37"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="37"/>
-      <c r="G98" s="38"/>
-      <c r="H98" s="38"/>
+      <c r="D98" s="62"/>
+      <c r="E98" s="62"/>
+      <c r="F98" s="62"/>
+      <c r="G98" s="70"/>
+      <c r="H98" s="70"/>
     </row>
     <row r="99" spans="1:35" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A99"/>
       <c r="B99"/>
-      <c r="C99" s="37" t="s">
+      <c r="C99" s="62" t="s">
         <v>49</v>
       </c>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="37"/>
-      <c r="G99" s="38"/>
-      <c r="H99" s="38"/>
+      <c r="D99" s="62"/>
+      <c r="E99" s="62"/>
+      <c r="F99" s="62"/>
+      <c r="G99" s="70"/>
+      <c r="H99" s="70"/>
     </row>
     <row r="100" spans="1:35" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A100"/>
       <c r="B100"/>
-      <c r="C100" s="37" t="s">
+      <c r="C100" s="62" t="s">
         <v>50</v>
       </c>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="37"/>
-      <c r="G100" s="38"/>
-      <c r="H100" s="38"/>
+      <c r="D100" s="62"/>
+      <c r="E100" s="62"/>
+      <c r="F100" s="62"/>
+      <c r="G100" s="70"/>
+      <c r="H100" s="70"/>
     </row>
     <row r="101" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C101" s="37" t="s">
+      <c r="C101" s="62" t="s">
         <v>51</v>
       </c>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="37"/>
-      <c r="G101" s="38"/>
-      <c r="H101" s="38"/>
+      <c r="D101" s="62"/>
+      <c r="E101" s="62"/>
+      <c r="F101" s="62"/>
+      <c r="G101" s="70"/>
+      <c r="H101" s="70"/>
       <c r="I101"/>
       <c r="J101"/>
       <c r="K101"/>
@@ -5167,14 +5167,14 @@
     <row r="102" spans="1:35" s="7" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A102" s="8"/>
       <c r="B102" s="8"/>
-      <c r="C102" s="37" t="s">
+      <c r="C102" s="62" t="s">
         <v>52</v>
       </c>
-      <c r="D102" s="37"/>
-      <c r="E102" s="37"/>
-      <c r="F102" s="37"/>
-      <c r="G102" s="38"/>
-      <c r="H102" s="38"/>
+      <c r="D102" s="62"/>
+      <c r="E102" s="62"/>
+      <c r="F102" s="62"/>
+      <c r="G102" s="70"/>
+      <c r="H102" s="70"/>
     </row>
     <row r="103" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A103" s="1"/>
@@ -5214,41 +5214,41 @@
     <row r="104" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A104" s="11"/>
       <c r="B104" s="11"/>
-      <c r="C104" s="70" t="s">
+      <c r="C104" s="37" t="s">
         <v>54</v>
       </c>
-      <c r="D104" s="70"/>
-      <c r="E104" s="70"/>
-      <c r="F104" s="70"/>
-      <c r="G104" s="70"/>
-      <c r="H104" s="70"/>
-      <c r="I104" s="70"/>
-      <c r="J104" s="70"/>
-      <c r="K104" s="70"/>
-      <c r="L104" s="70"/>
-      <c r="M104" s="70"/>
-      <c r="N104" s="70"/>
-      <c r="O104" s="70"/>
-      <c r="P104" s="70"/>
-      <c r="Q104" s="70"/>
-      <c r="R104" s="70"/>
-      <c r="S104" s="70"/>
-      <c r="T104" s="70"/>
-      <c r="U104" s="70"/>
-      <c r="V104" s="70"/>
-      <c r="W104" s="70"/>
-      <c r="X104" s="70"/>
-      <c r="Y104" s="70"/>
-      <c r="Z104" s="70"/>
-      <c r="AA104" s="70"/>
-      <c r="AB104" s="70"/>
-      <c r="AC104" s="70"/>
-      <c r="AD104" s="70"/>
-      <c r="AE104" s="70"/>
-      <c r="AF104" s="70"/>
-      <c r="AG104" s="70"/>
-      <c r="AH104" s="70"/>
-      <c r="AI104" s="70"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="37"/>
+      <c r="G104" s="37"/>
+      <c r="H104" s="37"/>
+      <c r="I104" s="37"/>
+      <c r="J104" s="37"/>
+      <c r="K104" s="37"/>
+      <c r="L104" s="37"/>
+      <c r="M104" s="37"/>
+      <c r="N104" s="37"/>
+      <c r="O104" s="37"/>
+      <c r="P104" s="37"/>
+      <c r="Q104" s="37"/>
+      <c r="R104" s="37"/>
+      <c r="S104" s="37"/>
+      <c r="T104" s="37"/>
+      <c r="U104" s="37"/>
+      <c r="V104" s="37"/>
+      <c r="W104" s="37"/>
+      <c r="X104" s="37"/>
+      <c r="Y104" s="37"/>
+      <c r="Z104" s="37"/>
+      <c r="AA104" s="37"/>
+      <c r="AB104" s="37"/>
+      <c r="AC104" s="37"/>
+      <c r="AD104" s="37"/>
+      <c r="AE104" s="37"/>
+      <c r="AF104" s="37"/>
+      <c r="AG104" s="37"/>
+      <c r="AH104" s="37"/>
+      <c r="AI104" s="37"/>
     </row>
     <row r="105" spans="1:35" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A105" s="11"/>
@@ -5731,18 +5731,29 @@
     </row>
   </sheetData>
   <mergeCells count="55">
-    <mergeCell ref="C104:AI104"/>
-    <mergeCell ref="B84:AH84"/>
-    <mergeCell ref="E74:E83"/>
-    <mergeCell ref="AB58:AB67"/>
-    <mergeCell ref="AC58:AC67"/>
-    <mergeCell ref="D58:D67"/>
-    <mergeCell ref="AE58:AE67"/>
-    <mergeCell ref="AF58:AF67"/>
-    <mergeCell ref="AG58:AG67"/>
-    <mergeCell ref="W58:W67"/>
-    <mergeCell ref="AD58:AD67"/>
-    <mergeCell ref="D74:D83"/>
+    <mergeCell ref="C100:F100"/>
+    <mergeCell ref="G100:H100"/>
+    <mergeCell ref="C101:F101"/>
+    <mergeCell ref="G101:H101"/>
+    <mergeCell ref="C102:F102"/>
+    <mergeCell ref="G102:H102"/>
+    <mergeCell ref="C97:F97"/>
+    <mergeCell ref="G97:H97"/>
+    <mergeCell ref="C98:F98"/>
+    <mergeCell ref="G98:H98"/>
+    <mergeCell ref="C99:F99"/>
+    <mergeCell ref="G99:H99"/>
+    <mergeCell ref="C93:F93"/>
+    <mergeCell ref="C94:F94"/>
+    <mergeCell ref="C95:F95"/>
+    <mergeCell ref="C96:F96"/>
+    <mergeCell ref="G90:H90"/>
+    <mergeCell ref="G91:H91"/>
+    <mergeCell ref="G92:H92"/>
+    <mergeCell ref="G93:H93"/>
+    <mergeCell ref="G94:H94"/>
+    <mergeCell ref="G95:H95"/>
+    <mergeCell ref="G96:H96"/>
     <mergeCell ref="C2:AH2"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C71:C72"/>
@@ -5759,33 +5770,22 @@
     <mergeCell ref="B52:AH52"/>
     <mergeCell ref="B57:AI57"/>
     <mergeCell ref="C68:AI68"/>
+    <mergeCell ref="C104:AI104"/>
+    <mergeCell ref="B84:AH84"/>
+    <mergeCell ref="E74:E83"/>
+    <mergeCell ref="AB58:AB67"/>
+    <mergeCell ref="AC58:AC67"/>
+    <mergeCell ref="D58:D67"/>
+    <mergeCell ref="AE58:AE67"/>
+    <mergeCell ref="AF58:AF67"/>
+    <mergeCell ref="AG58:AG67"/>
+    <mergeCell ref="W58:W67"/>
+    <mergeCell ref="AD58:AD67"/>
+    <mergeCell ref="D74:D83"/>
     <mergeCell ref="C89:H89"/>
     <mergeCell ref="C90:F90"/>
     <mergeCell ref="C91:F91"/>
     <mergeCell ref="C92:F92"/>
-    <mergeCell ref="C93:F93"/>
-    <mergeCell ref="C94:F94"/>
-    <mergeCell ref="C95:F95"/>
-    <mergeCell ref="C96:F96"/>
-    <mergeCell ref="G90:H90"/>
-    <mergeCell ref="G91:H91"/>
-    <mergeCell ref="G92:H92"/>
-    <mergeCell ref="G93:H93"/>
-    <mergeCell ref="G94:H94"/>
-    <mergeCell ref="G95:H95"/>
-    <mergeCell ref="G96:H96"/>
-    <mergeCell ref="C97:F97"/>
-    <mergeCell ref="G97:H97"/>
-    <mergeCell ref="C98:F98"/>
-    <mergeCell ref="G98:H98"/>
-    <mergeCell ref="C99:F99"/>
-    <mergeCell ref="G99:H99"/>
-    <mergeCell ref="C100:F100"/>
-    <mergeCell ref="G100:H100"/>
-    <mergeCell ref="C101:F101"/>
-    <mergeCell ref="G101:H101"/>
-    <mergeCell ref="C102:F102"/>
-    <mergeCell ref="G102:H102"/>
   </mergeCells>
   <phoneticPr fontId="11" type="noConversion"/>
   <hyperlinks>

</xml_diff>